<commit_message>
added log files and modified python files
</commit_message>
<xml_diff>
--- a/Final report.xlsx
+++ b/Final report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8772"/>
+    <workbookView windowWidth="22368" windowHeight="9144"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="106">
   <si>
     <t>服务器、用户名</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>https://www.facebook.com/groups/5106606936106939/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Crypto currency Ethereum Blockchain Dogecoin Bitcoin NFT</t>
@@ -339,11 +342,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -369,20 +372,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -395,66 +384,6 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -474,7 +403,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -490,8 +418,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -500,6 +466,43 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -520,7 +523,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,7 +649,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,115 +685,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,43 +697,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -711,54 +714,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -779,10 +734,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -793,6 +746,36 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -811,15 +794,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -828,136 +834,133 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -983,7 +986,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1337,18 +1340,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U$1:U$1048576"/>
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.1111111111111" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.1111111111111" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.6666666666667" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.4444444444444" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.1111111111111" style="2" customWidth="1"/>
     <col min="5" max="5" width="6.44444444444444" style="2" customWidth="1"/>
     <col min="6" max="6" width="2.22222222222222" customWidth="1"/>
     <col min="7" max="7" width="3.44444444444444" customWidth="1"/>
@@ -1362,13 +1365,11 @@
     <col min="15" max="17" width="6.11111111111111" customWidth="1"/>
     <col min="18" max="18" width="6.88888888888889" customWidth="1"/>
     <col min="19" max="19" width="6.44444444444444" customWidth="1"/>
-    <col min="20" max="20" width="9.11111111111111" customWidth="1"/>
-    <col min="21" max="21" width="10.3333333333333" customWidth="1"/>
-    <col min="22" max="22" width="11.4444444444444" customWidth="1"/>
-    <col min="23" max="23" width="27.1111111111111" customWidth="1"/>
+    <col min="20" max="20" width="7.33333333333333" customWidth="1"/>
+    <col min="21" max="23" width="6.88888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="28" customHeight="1" spans="1:23">
+    <row r="1" s="1" customFormat="1" ht="28" customHeight="1" spans="1:24">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1435,11 +1436,14 @@
       <c r="V1" s="7">
         <v>44874</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="7">
+        <v>44875</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:24">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1507,10 +1511,13 @@
         <v>15300</v>
       </c>
       <c r="W2">
+        <v>15400</v>
+      </c>
+      <c r="X2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:24">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1578,10 +1585,13 @@
         <v>1400</v>
       </c>
       <c r="W3">
+        <v>1400</v>
+      </c>
+      <c r="X3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:24">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1649,10 +1659,13 @@
         <v>14700</v>
       </c>
       <c r="W4">
+        <v>14800</v>
+      </c>
+      <c r="X4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:24">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1720,10 +1733,13 @@
         <v>14700</v>
       </c>
       <c r="W5">
+        <v>14700</v>
+      </c>
+      <c r="X5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:24">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1791,10 +1807,13 @@
         <v>14600</v>
       </c>
       <c r="W6">
+        <v>14700</v>
+      </c>
+      <c r="X6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:24">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1862,10 +1881,13 @@
         <v>14600</v>
       </c>
       <c r="W7">
+        <v>14700</v>
+      </c>
+      <c r="X7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:24">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1933,10 +1955,13 @@
         <v>14400</v>
       </c>
       <c r="W8">
+        <v>14500</v>
+      </c>
+      <c r="X8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:24">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -2004,10 +2029,13 @@
         <v>14400</v>
       </c>
       <c r="W9">
+        <v>14500</v>
+      </c>
+      <c r="X9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:24">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2075,10 +2103,13 @@
         <v>14300</v>
       </c>
       <c r="W10">
+        <v>14300</v>
+      </c>
+      <c r="X10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" ht="86.4" spans="1:23">
+    <row r="11" ht="86.4" spans="1:24">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2146,10 +2177,13 @@
         <v>14200</v>
       </c>
       <c r="W11">
+        <v>14300</v>
+      </c>
+      <c r="X11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:24">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -2217,10 +2251,13 @@
         <v>1300</v>
       </c>
       <c r="W12">
+        <v>1300</v>
+      </c>
+      <c r="X12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:24">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2285,10 +2322,13 @@
         <v>13700</v>
       </c>
       <c r="W13">
+        <v>13800</v>
+      </c>
+      <c r="X13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" ht="100.8" spans="1:23">
+    <row r="14" ht="100.8" spans="1:24">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -2356,10 +2396,13 @@
         <v>12600</v>
       </c>
       <c r="W14">
+        <v>12600</v>
+      </c>
+      <c r="X14">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:24">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -2427,10 +2470,13 @@
         <v>12500</v>
       </c>
       <c r="W15">
+        <v>12600</v>
+      </c>
+      <c r="X15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:24">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -2498,10 +2544,13 @@
         <v>12500</v>
       </c>
       <c r="W16">
+        <v>12600</v>
+      </c>
+      <c r="X16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:24">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -2569,10 +2618,13 @@
         <v>12100</v>
       </c>
       <c r="W17">
+        <v>12200</v>
+      </c>
+      <c r="X17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:24">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -2640,10 +2692,13 @@
         <v>12100</v>
       </c>
       <c r="W18">
+        <v>12100</v>
+      </c>
+      <c r="X18">
         <v>5</v>
       </c>
     </row>
-    <row r="19" ht="115.2" spans="1:23">
+    <row r="19" ht="115.2" spans="1:24">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -2711,10 +2766,13 @@
         <v>1200</v>
       </c>
       <c r="W19">
+        <v>1200</v>
+      </c>
+      <c r="X19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:24">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -2782,10 +2840,13 @@
         <v>12000</v>
       </c>
       <c r="W20">
+        <v>12100</v>
+      </c>
+      <c r="X20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:24">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
@@ -2853,10 +2914,13 @@
         <v>11900</v>
       </c>
       <c r="W21">
+        <v>12000</v>
+      </c>
+      <c r="X21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:24">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -2924,10 +2988,13 @@
         <v>11900</v>
       </c>
       <c r="W22">
+        <v>12000</v>
+      </c>
+      <c r="X22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:24">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2995,10 +3062,13 @@
         <v>1200</v>
       </c>
       <c r="W23">
+        <v>1200</v>
+      </c>
+      <c r="X23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:24">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
@@ -3063,10 +3133,13 @@
         <v>15300</v>
       </c>
       <c r="W24">
+        <v>15300</v>
+      </c>
+      <c r="X24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:24">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -3131,10 +3204,13 @@
         <v>15100</v>
       </c>
       <c r="W25">
+        <v>15200</v>
+      </c>
+      <c r="X25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:24">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -3199,10 +3275,13 @@
         <v>1400</v>
       </c>
       <c r="W26">
+        <v>1400</v>
+      </c>
+      <c r="X26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:24">
       <c r="A27" s="2" t="s">
         <v>9</v>
       </c>
@@ -3267,10 +3346,13 @@
         <v>15100</v>
       </c>
       <c r="W27">
+        <v>15100</v>
+      </c>
+      <c r="X27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:24">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
@@ -3335,10 +3417,13 @@
         <v>15000</v>
       </c>
       <c r="W28">
+        <v>15100</v>
+      </c>
+      <c r="X28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:24">
       <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
@@ -3403,21 +3488,24 @@
         <v>15000</v>
       </c>
       <c r="W29">
+        <v>15100</v>
+      </c>
+      <c r="X29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:24">
       <c r="A30" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G30">
         <v>14</v>
@@ -3441,10 +3529,13 @@
         <v>270</v>
       </c>
       <c r="W30">
+        <v>275</v>
+      </c>
+      <c r="X30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:24">
       <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
@@ -3452,10 +3543,10 @@
         <v>13</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G31">
         <v>5</v>
@@ -3479,10 +3570,13 @@
         <v>2300</v>
       </c>
       <c r="W31">
+        <v>2400</v>
+      </c>
+      <c r="X31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:24">
       <c r="A32" s="2" t="s">
         <v>9</v>
       </c>
@@ -3490,10 +3584,10 @@
         <v>40</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G32">
         <v>15</v>
@@ -3517,10 +3611,13 @@
         <v>2300</v>
       </c>
       <c r="W32">
+        <v>2400</v>
+      </c>
+      <c r="X32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:24">
       <c r="A33" s="2" t="s">
         <v>9</v>
       </c>
@@ -3528,10 +3625,10 @@
         <v>62</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G33">
         <v>21</v>
@@ -3540,7 +3637,7 @@
         <v>1</v>
       </c>
       <c r="P33" s="8">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="Q33">
         <v>201</v>
@@ -3555,10 +3652,13 @@
         <v>2300</v>
       </c>
       <c r="W33">
+        <v>2400</v>
+      </c>
+      <c r="X33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:24">
       <c r="A34" s="2" t="s">
         <v>9</v>
       </c>
@@ -3566,10 +3666,10 @@
         <v>83</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -3593,6 +3693,9 @@
         <v>2300</v>
       </c>
       <c r="W34">
+        <v>2400</v>
+      </c>
+      <c r="X34">
         <v>0</v>
       </c>
     </row>
@@ -3644,7 +3747,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X24" sqref="X24"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3661,7 +3764,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X24" sqref="X24"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
added new python files, modified old python files, and added log files
</commit_message>
<xml_diff>
--- a/Final report.xlsx
+++ b/Final report.xlsx
@@ -1337,10 +1337,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AA34"/>
+  <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="Z37" sqref="Z37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1363,10 +1363,10 @@
     <col min="18" max="18" width="6.88888888888889" customWidth="1"/>
     <col min="19" max="19" width="6.44444444444444" customWidth="1"/>
     <col min="20" max="20" width="7.33333333333333" customWidth="1"/>
-    <col min="21" max="26" width="6.88888888888889" customWidth="1"/>
+    <col min="21" max="27" width="6.88888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="28" customHeight="1" spans="1:27">
+    <row r="1" s="1" customFormat="1" ht="28" customHeight="1" spans="1:28">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1445,11 +1445,14 @@
       <c r="Z1" s="7">
         <v>44879</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="7">
+        <v>44880</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:28">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1529,10 +1532,13 @@
         <v>15994</v>
       </c>
       <c r="AA2">
-        <v>15</v>
+        <v>17035</v>
+      </c>
+      <c r="AB2">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:28">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1612,10 +1618,13 @@
         <v>1498</v>
       </c>
       <c r="AA3">
+        <v>1527</v>
+      </c>
+      <c r="AB3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:28">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1695,10 +1704,13 @@
         <v>15850</v>
       </c>
       <c r="AA4">
-        <v>29</v>
+        <v>16211</v>
+      </c>
+      <c r="AB4">
+        <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:28">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1778,10 +1790,13 @@
         <v>15771</v>
       </c>
       <c r="AA5">
+        <v>16182</v>
+      </c>
+      <c r="AB5">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:28">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1861,10 +1876,13 @@
         <v>15673</v>
       </c>
       <c r="AA6">
-        <v>21</v>
+        <v>16128</v>
+      </c>
+      <c r="AB6">
+        <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:28">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1944,10 +1962,13 @@
         <v>15533</v>
       </c>
       <c r="AA7">
-        <v>16</v>
+        <v>16094</v>
+      </c>
+      <c r="AB7">
+        <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:28">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -2027,10 +2048,13 @@
         <v>15319</v>
       </c>
       <c r="AA8">
+        <v>15888</v>
+      </c>
+      <c r="AB8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:28">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -2110,10 +2134,13 @@
         <v>14924</v>
       </c>
       <c r="AA9">
+        <v>15843</v>
+      </c>
+      <c r="AB9">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:28">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2193,10 +2220,13 @@
         <v>15184</v>
       </c>
       <c r="AA10">
-        <v>26</v>
+        <v>15762</v>
+      </c>
+      <c r="AB10">
+        <v>27</v>
       </c>
     </row>
-    <row r="11" ht="86.4" spans="1:27">
+    <row r="11" ht="86.4" spans="1:28">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2276,10 +2306,13 @@
         <v>15112</v>
       </c>
       <c r="AA11">
-        <v>16</v>
+        <v>15686</v>
+      </c>
+      <c r="AB11">
+        <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:28">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -2359,10 +2392,13 @@
         <v>1340</v>
       </c>
       <c r="AA12">
+        <v>1457</v>
+      </c>
+      <c r="AB12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:28">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2439,10 +2475,13 @@
         <v>14547</v>
       </c>
       <c r="AA13">
-        <v>7</v>
+        <v>15129</v>
+      </c>
+      <c r="AB13">
+        <v>8</v>
       </c>
     </row>
-    <row r="14" ht="100.8" spans="1:27">
+    <row r="14" ht="100.8" spans="1:28">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -2522,10 +2561,13 @@
         <v>13407</v>
       </c>
       <c r="AA14">
-        <v>9</v>
+        <v>14003</v>
+      </c>
+      <c r="AB14">
+        <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:28">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -2605,10 +2647,13 @@
         <v>13330</v>
       </c>
       <c r="AA15">
+        <v>13930</v>
+      </c>
+      <c r="AB15">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:28">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -2688,10 +2733,13 @@
         <v>12930</v>
       </c>
       <c r="AA16">
-        <v>6</v>
+        <v>13871</v>
+      </c>
+      <c r="AB16">
+        <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:28">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -2771,10 +2819,13 @@
         <v>12534</v>
       </c>
       <c r="AA17">
+        <v>12534</v>
+      </c>
+      <c r="AB17">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:28">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -2854,10 +2905,13 @@
         <v>12866</v>
       </c>
       <c r="AA18">
+        <v>13414</v>
+      </c>
+      <c r="AB18">
         <v>9</v>
       </c>
     </row>
-    <row r="19" ht="115.2" spans="1:27">
+    <row r="19" ht="115.2" spans="1:28">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -2937,10 +2991,13 @@
         <v>1210</v>
       </c>
       <c r="AA19">
-        <v>1</v>
+        <v>1307</v>
+      </c>
+      <c r="AB19">
+        <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:28">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -3020,10 +3077,13 @@
         <v>12415</v>
       </c>
       <c r="AA20">
-        <v>4</v>
+        <v>13303</v>
+      </c>
+      <c r="AB20">
+        <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:28">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
@@ -3103,10 +3163,13 @@
         <v>12700</v>
       </c>
       <c r="AA21">
+        <v>13211</v>
+      </c>
+      <c r="AB21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:28">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -3186,10 +3249,13 @@
         <v>12656</v>
       </c>
       <c r="AA22">
-        <v>30</v>
+        <v>13165</v>
+      </c>
+      <c r="AB22">
+        <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:28">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -3269,10 +3335,13 @@
         <v>1196</v>
       </c>
       <c r="AA23">
+        <v>1298</v>
+      </c>
+      <c r="AB23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:28">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
@@ -3349,10 +3418,13 @@
         <v>16046</v>
       </c>
       <c r="AA24">
+        <v>16570</v>
+      </c>
+      <c r="AB24">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:28">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -3429,10 +3501,13 @@
         <v>15902</v>
       </c>
       <c r="AA25">
+        <v>16411</v>
+      </c>
+      <c r="AB25">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:28">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -3509,10 +3584,13 @@
         <v>1411</v>
       </c>
       <c r="AA26">
+        <v>1511</v>
+      </c>
+      <c r="AB26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:28">
       <c r="A27" s="2" t="s">
         <v>9</v>
       </c>
@@ -3589,10 +3667,13 @@
         <v>15403</v>
       </c>
       <c r="AA27">
-        <v>16</v>
+        <v>16310</v>
+      </c>
+      <c r="AB27">
+        <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:28">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
@@ -3669,10 +3750,13 @@
         <v>15736</v>
       </c>
       <c r="AA28">
-        <v>4</v>
+        <v>16124</v>
+      </c>
+      <c r="AB28">
+        <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:28">
       <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
@@ -3749,10 +3833,13 @@
         <v>15772</v>
       </c>
       <c r="AA29">
+        <v>16200</v>
+      </c>
+      <c r="AB29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:28">
       <c r="A30" s="2" t="s">
         <v>9</v>
       </c>
@@ -3799,11 +3886,13 @@
         <v>341</v>
       </c>
       <c r="AA30">
-        <f>SUM(AA31:AA31)</f>
+        <v>398</v>
+      </c>
+      <c r="AB30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:28">
       <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
@@ -3850,11 +3939,13 @@
         <v>2618</v>
       </c>
       <c r="AA31">
-        <f>SUM(AA32:AA32)</f>
+        <v>3534</v>
+      </c>
+      <c r="AB31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:28">
       <c r="A32" s="2" t="s">
         <v>9</v>
       </c>
@@ -3901,11 +3992,13 @@
         <v>3007</v>
       </c>
       <c r="AA32">
-        <f>SUM(AA33:AB33)</f>
+        <v>3514</v>
+      </c>
+      <c r="AB32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:28">
       <c r="A33" s="2" t="s">
         <v>9</v>
       </c>
@@ -3952,11 +4045,13 @@
         <v>2665</v>
       </c>
       <c r="AA33">
-        <f>SUM(AA34:AB34)</f>
+        <v>3504</v>
+      </c>
+      <c r="AB33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:28">
       <c r="A34" s="2" t="s">
         <v>9</v>
       </c>
@@ -4003,6 +4098,9 @@
         <v>2585</v>
       </c>
       <c r="AA34">
+        <v>3492</v>
+      </c>
+      <c r="AB34">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new python files and logs file
</commit_message>
<xml_diff>
--- a/Final report.xlsx
+++ b/Final report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9144"/>
+    <workbookView windowWidth="23040" windowHeight="9215"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,13 +339,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd\-mmm"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,7 +355,72 @@
     </font>
     <font>
       <sz val="14"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -369,16 +434,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -400,13 +480,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -415,26 +488,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -454,81 +511,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -538,7 +532,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,7 +556,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,13 +568,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,7 +586,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,67 +664,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -670,37 +694,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -711,6 +717,71 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -733,61 +804,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -800,164 +817,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -968,25 +974,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1337,10 +1343,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AB34"/>
+  <dimension ref="A1:AB36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1348,38 +1354,39 @@
     <col min="1" max="1" width="19.1111111111111" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.1111111111111" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.4444444444444" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.1111111111111" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.1111111111111" style="2" customWidth="1"/>
     <col min="5" max="5" width="6.44444444444444" style="2" customWidth="1"/>
-    <col min="6" max="6" width="2.22222222222222" customWidth="1"/>
-    <col min="7" max="7" width="3.44444444444444" customWidth="1"/>
-    <col min="8" max="8" width="4.11111111111111" customWidth="1"/>
-    <col min="9" max="9" width="5.66666666666667" customWidth="1"/>
-    <col min="10" max="10" width="5.22222222222222" customWidth="1"/>
-    <col min="11" max="11" width="5.33333333333333" customWidth="1"/>
-    <col min="12" max="12" width="5.11111111111111" customWidth="1"/>
-    <col min="13" max="13" width="5.22222222222222" customWidth="1"/>
-    <col min="14" max="14" width="5.88888888888889" customWidth="1"/>
-    <col min="15" max="17" width="6.11111111111111" customWidth="1"/>
-    <col min="18" max="18" width="6.88888888888889" customWidth="1"/>
-    <col min="19" max="19" width="6.44444444444444" customWidth="1"/>
-    <col min="20" max="20" width="7.33333333333333" customWidth="1"/>
-    <col min="21" max="27" width="6.88888888888889" customWidth="1"/>
+    <col min="6" max="6" width="2.22222222222222" style="3" customWidth="1"/>
+    <col min="7" max="7" width="3.44444444444444" style="3" customWidth="1"/>
+    <col min="8" max="8" width="4.11111111111111" style="3" customWidth="1"/>
+    <col min="9" max="9" width="5.66666666666667" style="3" customWidth="1"/>
+    <col min="10" max="10" width="5.22222222222222" style="3" customWidth="1"/>
+    <col min="11" max="11" width="5.33333333333333" style="3" customWidth="1"/>
+    <col min="12" max="12" width="5.11111111111111" style="3" customWidth="1"/>
+    <col min="13" max="13" width="5.22222222222222" style="3" customWidth="1"/>
+    <col min="14" max="14" width="5.88888888888889" style="3" customWidth="1"/>
+    <col min="15" max="17" width="6.11111111111111" style="3" customWidth="1"/>
+    <col min="18" max="18" width="6.88888888888889" style="3" customWidth="1"/>
+    <col min="19" max="19" width="6.44444444444444" style="3" customWidth="1"/>
+    <col min="20" max="20" width="7.33333333333333" style="3" customWidth="1"/>
+    <col min="21" max="27" width="6.88888888888889" style="3" customWidth="1"/>
+    <col min="28" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="28" customHeight="1" spans="1:28">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1391,61 +1398,61 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7">
+      <c r="I1" s="8">
         <v>44858</v>
       </c>
-      <c r="J1" s="7">
+      <c r="J1" s="8">
         <v>44859</v>
       </c>
-      <c r="K1" s="7">
+      <c r="K1" s="8">
         <v>44860</v>
       </c>
-      <c r="L1" s="7">
+      <c r="L1" s="8">
         <v>44861</v>
       </c>
-      <c r="M1" s="7">
+      <c r="M1" s="8">
         <v>44862</v>
       </c>
-      <c r="N1" s="7">
+      <c r="N1" s="8">
         <v>44865</v>
       </c>
-      <c r="O1" s="7">
+      <c r="O1" s="8">
         <v>44866</v>
       </c>
-      <c r="P1" s="7">
+      <c r="P1" s="8">
         <v>44867</v>
       </c>
-      <c r="Q1" s="7">
+      <c r="Q1" s="8">
         <v>44868</v>
       </c>
-      <c r="R1" s="7">
+      <c r="R1" s="8">
         <v>44869</v>
       </c>
-      <c r="S1" s="7">
+      <c r="S1" s="8">
         <v>44870</v>
       </c>
-      <c r="T1" s="7">
+      <c r="T1" s="8">
         <v>44872</v>
       </c>
-      <c r="U1" s="7">
+      <c r="U1" s="8">
         <v>44873</v>
       </c>
-      <c r="V1" s="7">
+      <c r="V1" s="8">
         <v>44874</v>
       </c>
-      <c r="W1" s="7">
+      <c r="W1" s="8">
         <v>44875</v>
       </c>
-      <c r="X1" s="7">
+      <c r="X1" s="8">
         <v>44876</v>
       </c>
-      <c r="Y1" s="7">
+      <c r="Y1" s="8">
         <v>44877</v>
       </c>
-      <c r="Z1" s="7">
+      <c r="Z1" s="8">
         <v>44879</v>
       </c>
-      <c r="AA1" s="7">
+      <c r="AA1" s="8">
         <v>44880</v>
       </c>
       <c r="AB1" s="1" t="s">
@@ -1453,2656 +1460,2662 @@
       </c>
     </row>
     <row r="2" spans="1:28">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="2">
         <v>3800</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>18</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>11</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>5800</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <v>7200</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>7200</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <v>7200</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="3">
         <v>8600</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="3">
         <v>10900</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="3">
         <v>12300</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="3">
         <v>12900</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="3">
         <v>13100</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="3">
         <v>13500</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="3">
         <v>13800</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="3">
         <v>14300</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="3">
         <v>14800</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="3">
         <v>15300</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="3">
         <v>15400</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="3">
         <v>15700</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="3">
         <v>15994</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="3">
         <v>15994</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="3">
         <v>17035</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="3">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:28">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="2">
         <v>236</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>13</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>3</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>380</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>476</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>479</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <v>538</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="3">
         <v>632</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="3">
         <v>847</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="3">
         <v>1000</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="3">
         <v>1100</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="3">
         <v>1100</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="3">
         <v>1100</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="3">
         <v>1200</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="3">
         <v>1200</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="3">
         <v>1300</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="3">
         <v>1400</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="3">
         <v>1400</v>
       </c>
-      <c r="X3">
+      <c r="X3" s="3">
         <v>1400</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="3">
         <v>1409</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="3">
         <v>1498</v>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="3">
         <v>1527</v>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:28">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="2">
         <v>3200</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>8</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>49</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>5300</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>6500</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>6700</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <v>7200</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="3">
         <v>8100</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="3">
         <v>9900</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="3">
         <v>11700</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="3">
         <v>12100</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="3">
         <v>12500</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="3">
         <v>12900</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="3">
         <v>13000</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="3">
         <v>13600</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="3">
         <v>14000</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="3">
         <v>14700</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="3">
         <v>14800</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="3">
         <v>15100</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="3">
         <v>15156</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="3">
         <v>15850</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="3">
         <v>16211</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="3">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:28">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="2">
         <v>3200</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>1</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>71</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>7</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>5300</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <v>6500</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <v>6700</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="3">
         <v>7200</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="3">
         <v>8100</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="3">
         <v>9700</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="3">
         <v>11700</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="3">
         <v>12000</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="3">
         <v>12500</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="3">
         <v>12900</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="3">
         <v>13000</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="3">
         <v>13600</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="3">
         <v>13900</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="3">
         <v>14700</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="3">
         <v>14700</v>
       </c>
-      <c r="X5">
+      <c r="X5" s="3">
         <v>15100</v>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="3">
         <v>15123</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="3">
         <v>15771</v>
       </c>
-      <c r="AA5">
+      <c r="AA5" s="3">
         <v>16182</v>
       </c>
-      <c r="AB5">
+      <c r="AB5" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:28">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="2">
         <v>3100</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>37</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>64</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <v>5200</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="3">
         <v>6300</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="3">
         <v>6700</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="3">
         <v>7100</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="3">
         <v>8000</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="3">
         <v>9800</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="3">
         <v>11600</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="3">
         <v>11900</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="3">
         <v>12400</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="3">
         <v>12800</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="3">
         <v>12900</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="3">
         <v>13500</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="3">
         <v>13800</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="3">
         <v>14600</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="3">
         <v>14700</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="3">
         <v>15100</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="3">
         <v>15071</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="3">
         <v>15673</v>
       </c>
-      <c r="AA6">
+      <c r="AA6" s="3">
         <v>16128</v>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="3">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:28">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="2">
         <v>3000</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>23</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>22</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <v>5200</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="3">
         <v>6200</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="3">
         <v>6500</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="3">
         <v>7000</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="3">
         <v>7900</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="3">
         <v>9600</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="3">
         <v>11500</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="3">
         <v>11800</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="3">
         <v>12400</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="3">
         <v>12800</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="3">
         <v>12900</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="3">
         <v>13500</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="3">
         <v>13800</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="3">
         <v>14600</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="3">
         <v>14700</v>
       </c>
-      <c r="X7">
+      <c r="X7" s="3">
         <v>15000</v>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="3">
         <v>15040</v>
       </c>
-      <c r="Z7">
+      <c r="Z7" s="3">
         <v>15533</v>
       </c>
-      <c r="AA7">
+      <c r="AA7" s="3">
         <v>16094</v>
       </c>
-      <c r="AB7">
+      <c r="AB7" s="3">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:28">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="2">
         <v>2900</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>59</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>55</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="3">
         <v>5000</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="3">
         <v>6100</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="3">
         <v>6400</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="3">
         <v>6900</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="3">
         <v>7800</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="3">
         <v>9400</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="3">
         <v>11200</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="3">
         <v>11600</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="3">
         <v>12200</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="3">
         <v>12600</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="3">
         <v>12700</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="3">
         <v>13300</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="3">
         <v>13600</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="3">
         <v>14400</v>
       </c>
-      <c r="W8">
+      <c r="W8" s="3">
         <v>14500</v>
       </c>
-      <c r="X8">
+      <c r="X8" s="3">
         <v>14800</v>
       </c>
-      <c r="Y8">
+      <c r="Y8" s="3">
         <v>14834</v>
       </c>
-      <c r="Z8">
+      <c r="Z8" s="3">
         <v>15319</v>
       </c>
-      <c r="AA8">
+      <c r="AA8" s="3">
         <v>15888</v>
       </c>
-      <c r="AB8">
+      <c r="AB8" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:28">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="2">
         <v>2800</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>14</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>12</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="3">
         <v>5000</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="3">
         <v>6000</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="3">
         <v>6300</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="3">
         <v>6800</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="3">
         <v>7700</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="3">
         <v>9300</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="3">
         <v>11000</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="3">
         <v>11600</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="3">
         <v>12200</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="3">
         <v>12600</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="3">
         <v>12700</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="3">
         <v>13300</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="3">
         <v>13500</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="3">
         <v>14400</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="3">
         <v>14500</v>
       </c>
-      <c r="X9">
+      <c r="X9" s="3">
         <v>14800</v>
       </c>
-      <c r="Y9">
+      <c r="Y9" s="3">
         <v>14924</v>
       </c>
-      <c r="Z9">
+      <c r="Z9" s="3">
         <v>14924</v>
       </c>
-      <c r="AA9">
+      <c r="AA9" s="3">
         <v>15843</v>
       </c>
-      <c r="AB9">
+      <c r="AB9" s="3">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:28">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E10" s="2">
         <v>2800</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>1</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>5</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>45</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="3">
         <v>4900</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="3">
         <v>6000</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="3">
         <v>6300</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="3">
         <v>6800</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="3">
         <v>7400</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="3">
         <v>9100</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="3">
         <v>10800</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="3">
         <v>11400</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="3">
         <v>12100</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="3">
         <v>12500</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="3">
         <v>12600</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="3">
         <v>13200</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="3">
         <v>13400</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="3">
         <v>14300</v>
       </c>
-      <c r="W10">
+      <c r="W10" s="3">
         <v>14300</v>
       </c>
-      <c r="X10">
+      <c r="X10" s="3">
         <v>14700</v>
       </c>
-      <c r="Y10">
+      <c r="Y10" s="3">
         <v>14700</v>
       </c>
-      <c r="Z10">
+      <c r="Z10" s="3">
         <v>15184</v>
       </c>
-      <c r="AA10">
+      <c r="AA10" s="3">
         <v>15762</v>
       </c>
-      <c r="AB10">
+      <c r="AB10" s="3">
         <v>27</v>
       </c>
     </row>
-    <row r="11" ht="86.4" spans="1:28">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:28">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="6" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="2">
         <v>2700</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>1</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>15</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="3">
         <v>4900</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="3">
         <v>5900</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="3">
         <v>6300</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="3">
         <v>6700</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="3">
         <v>7300</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="3">
         <v>9100</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="3">
         <v>10700</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="3">
         <v>11400</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="3">
         <v>12000</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="3">
         <v>12400</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="3">
         <v>12500</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="3">
         <v>13100</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="3">
         <v>13400</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="3">
         <v>14200</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="3">
         <v>14300</v>
       </c>
-      <c r="X11">
+      <c r="X11" s="3">
         <v>14600</v>
       </c>
-      <c r="Y11">
+      <c r="Y11" s="3">
         <v>14644</v>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="3">
         <v>15112</v>
       </c>
-      <c r="AA11">
+      <c r="AA11" s="3">
         <v>15686</v>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="3">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:28">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="2">
         <v>151</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>1</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>21</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
         <v>296</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="3">
         <v>394</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="3">
         <v>417</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="3">
         <v>472</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="3">
         <v>531</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="3">
         <v>724</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="3">
         <v>881</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="3">
         <v>949</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="3">
         <v>1000</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="3">
         <v>1100</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="3">
         <v>1200</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="3">
         <v>1200</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="3">
         <v>1200</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="3">
         <v>1300</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="3">
         <v>1300</v>
       </c>
-      <c r="X12">
+      <c r="X12" s="3">
         <v>1300</v>
       </c>
-      <c r="Y12">
+      <c r="Y12" s="3">
         <v>1340</v>
       </c>
-      <c r="Z12">
+      <c r="Z12" s="3">
         <v>1340</v>
       </c>
-      <c r="AA12">
+      <c r="AA12" s="3">
         <v>1457</v>
       </c>
-      <c r="AB12">
+      <c r="AB12" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:28">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="6" t="s">
         <v>46</v>
       </c>
       <c r="E13" s="2">
         <v>2000</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>9</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>21</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="3">
         <v>5300</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="3">
         <v>5600</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="3">
         <v>6100</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="3">
         <v>6500</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="3">
         <v>8400</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="3">
         <v>10000</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="3">
         <v>10700</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="3">
         <v>11300</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="3">
         <v>11800</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="3">
         <v>11900</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="3">
         <v>12600</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="3">
         <v>12900</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="3">
         <v>13700</v>
       </c>
-      <c r="W13">
+      <c r="W13" s="3">
         <v>13800</v>
       </c>
-      <c r="X13">
+      <c r="X13" s="3">
         <v>14100</v>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="3">
         <v>14136</v>
       </c>
-      <c r="Z13">
+      <c r="Z13" s="3">
         <v>14547</v>
       </c>
-      <c r="AA13">
+      <c r="AA13" s="3">
         <v>15129</v>
       </c>
-      <c r="AB13">
+      <c r="AB13" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="14" ht="100.8" spans="1:28">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:28">
+      <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="6" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="2">
         <v>1100</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>1</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <v>1</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>15</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="3">
         <v>3200</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="3">
         <v>4300</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="3">
         <v>4400</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="3">
         <v>5100</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="3">
         <v>5300</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="3">
         <v>7400</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="3">
         <v>8800</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="3">
         <v>9700</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="3">
         <v>10300</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="3">
         <v>10700</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="3">
         <v>10800</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="3">
         <v>11500</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="3">
         <v>11700</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="3">
         <v>12600</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="3">
         <v>12600</v>
       </c>
-      <c r="X14">
+      <c r="X14" s="3">
         <v>13000</v>
       </c>
-      <c r="Y14">
+      <c r="Y14" s="3">
         <v>13028</v>
       </c>
-      <c r="Z14">
+      <c r="Z14" s="3">
         <v>13407</v>
       </c>
-      <c r="AA14">
+      <c r="AA14" s="3">
         <v>14003</v>
       </c>
-      <c r="AB14">
+      <c r="AB14" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:28">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="6" t="s">
         <v>52</v>
       </c>
       <c r="E15" s="2">
         <v>1100</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <v>1</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="3">
         <v>45</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>5</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="3">
         <v>3100</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="3">
         <v>4200</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="3">
         <v>4400</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="3">
         <v>5000</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="3">
         <v>5300</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="3">
         <v>7300</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="3">
         <v>8600</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="3">
         <v>9700</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="3">
         <v>10300</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="3">
         <v>10600</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="3">
         <v>10700</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="3">
         <v>11400</v>
       </c>
-      <c r="U15">
+      <c r="U15" s="3">
         <v>11700</v>
       </c>
-      <c r="V15">
+      <c r="V15" s="3">
         <v>12500</v>
       </c>
-      <c r="W15">
+      <c r="W15" s="3">
         <v>12600</v>
       </c>
-      <c r="X15">
+      <c r="X15" s="3">
         <v>12800</v>
       </c>
-      <c r="Y15">
+      <c r="Y15" s="3">
         <v>12966</v>
       </c>
-      <c r="Z15">
+      <c r="Z15" s="3">
         <v>13330</v>
       </c>
-      <c r="AA15">
+      <c r="AA15" s="3">
         <v>13930</v>
       </c>
-      <c r="AB15">
+      <c r="AB15" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:28">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E16" s="2">
         <v>1000</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>1</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>12</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>14</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="3">
         <v>3100</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="3">
         <v>4200</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="3">
         <v>4400</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="3">
         <v>5000</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="3">
         <v>5200</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="3">
         <v>7200</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="3">
         <v>8500</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="3">
         <v>9700</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="3">
         <v>10300</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="3">
         <v>10600</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="3">
         <v>10700</v>
       </c>
-      <c r="T16">
+      <c r="T16" s="3">
         <v>11400</v>
       </c>
-      <c r="U16">
+      <c r="U16" s="3">
         <v>11600</v>
       </c>
-      <c r="V16">
+      <c r="V16" s="3">
         <v>12500</v>
       </c>
-      <c r="W16">
+      <c r="W16" s="3">
         <v>12600</v>
       </c>
-      <c r="X16">
+      <c r="X16" s="3">
         <v>12800</v>
       </c>
-      <c r="Y16">
+      <c r="Y16" s="3">
         <v>12930</v>
       </c>
-      <c r="Z16">
+      <c r="Z16" s="3">
         <v>12930</v>
       </c>
-      <c r="AA16">
+      <c r="AA16" s="3">
         <v>13871</v>
       </c>
-      <c r="AB16">
+      <c r="AB16" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:28">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E17" s="2">
         <v>681</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>1</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>55</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="3">
         <v>59</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="3">
         <v>2500</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="3">
         <v>3800</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="3">
         <v>4000</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="3">
         <v>4600</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="3">
         <v>4800</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="3">
         <v>6900</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="3">
         <v>8100</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="3">
         <v>9300</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="3">
         <v>9900</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="3">
         <v>10200</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="3">
         <v>10300</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="3">
         <v>10900</v>
       </c>
-      <c r="U17">
+      <c r="U17" s="3">
         <v>11200</v>
       </c>
-      <c r="V17">
+      <c r="V17" s="3">
         <v>12100</v>
       </c>
-      <c r="W17">
+      <c r="W17" s="3">
         <v>12200</v>
       </c>
-      <c r="X17">
+      <c r="X17" s="3">
         <v>12400</v>
       </c>
-      <c r="Y17">
+      <c r="Y17" s="3">
         <v>12534</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="3">
         <v>12534</v>
       </c>
-      <c r="AA17">
+      <c r="AA17" s="3">
         <v>12534</v>
       </c>
-      <c r="AB17">
+      <c r="AB17" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:28">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E18" s="2">
         <v>674</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>1</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>22</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>23</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="3">
         <v>2300</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="3">
         <v>3800</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="3">
         <v>4000</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="3">
         <v>4600</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="3">
         <v>4800</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="3">
         <v>6800</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="3">
         <v>8000</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="3">
         <v>9200</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="3">
         <v>9900</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="3">
         <v>10100</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="3">
         <v>10300</v>
       </c>
-      <c r="T18">
+      <c r="T18" s="3">
         <v>10900</v>
       </c>
-      <c r="U18">
+      <c r="U18" s="3">
         <v>11100</v>
       </c>
-      <c r="V18">
+      <c r="V18" s="3">
         <v>12100</v>
       </c>
-      <c r="W18">
+      <c r="W18" s="3">
         <v>12100</v>
       </c>
-      <c r="X18">
+      <c r="X18" s="3">
         <v>12400</v>
       </c>
-      <c r="Y18">
+      <c r="Y18" s="3">
         <v>12510</v>
       </c>
-      <c r="Z18">
+      <c r="Z18" s="3">
         <v>12866</v>
       </c>
-      <c r="AA18">
+      <c r="AA18" s="3">
         <v>13414</v>
       </c>
-      <c r="AB18">
+      <c r="AB18" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="19" ht="115.2" spans="1:28">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:28">
+      <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="6" t="s">
         <v>64</v>
       </c>
       <c r="E19" s="2">
         <v>45</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>1</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>64</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>37</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="3">
         <v>148</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="3">
         <v>294</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="3">
         <v>299</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="3">
         <v>369</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="3">
         <v>395</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="3">
         <v>683</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="3">
         <v>704</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="3">
         <v>843</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="3">
         <v>908</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="3">
         <v>941</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="3">
         <v>956</v>
       </c>
-      <c r="T19">
+      <c r="T19" s="3">
         <v>1100</v>
       </c>
-      <c r="U19">
+      <c r="U19" s="3">
         <v>1100</v>
       </c>
-      <c r="V19">
+      <c r="V19" s="3">
         <v>1200</v>
       </c>
-      <c r="W19">
+      <c r="W19" s="3">
         <v>1200</v>
       </c>
-      <c r="X19">
+      <c r="X19" s="3">
         <v>1200</v>
       </c>
-      <c r="Y19">
+      <c r="Y19" s="3">
         <v>1210</v>
       </c>
-      <c r="Z19">
+      <c r="Z19" s="3">
         <v>1210</v>
       </c>
-      <c r="AA19">
+      <c r="AA19" s="3">
         <v>1307</v>
       </c>
-      <c r="AB19">
+      <c r="AB19" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:28">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E20" s="2">
         <v>631</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>1</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>7</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="3">
         <v>71</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="3">
         <v>2200</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="3">
         <v>3700</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="3">
         <v>3900</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="3">
         <v>4500</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="3">
         <v>4700</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="3">
         <v>6800</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="3">
         <v>7900</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="3">
         <v>9200</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="3">
         <v>9800</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="3">
         <v>10100</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="3">
         <v>10200</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="3">
         <v>10900</v>
       </c>
-      <c r="U20">
+      <c r="U20" s="3">
         <v>11000</v>
       </c>
-      <c r="V20">
+      <c r="V20" s="3">
         <v>12000</v>
       </c>
-      <c r="W20">
+      <c r="W20" s="3">
         <v>12100</v>
       </c>
-      <c r="X20">
+      <c r="X20" s="3">
         <v>12200</v>
       </c>
-      <c r="Y20">
+      <c r="Y20" s="3">
         <v>12415</v>
       </c>
-      <c r="Z20">
+      <c r="Z20" s="3">
         <v>12415</v>
       </c>
-      <c r="AA20">
+      <c r="AA20" s="3">
         <v>13303</v>
       </c>
-      <c r="AB20">
+      <c r="AB20" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:28">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="6" t="s">
         <v>70</v>
       </c>
       <c r="E21" s="2">
         <v>602</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>1</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>49</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="3">
         <v>8</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="3">
         <v>2200</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="3">
         <v>3700</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="3">
         <v>3800</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="3">
         <v>4500</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="3">
         <v>4700</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="3">
         <v>6700</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="3">
         <v>7800</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="3">
         <v>9100</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="3">
         <v>9700</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="3">
         <v>10000</v>
       </c>
-      <c r="S21">
+      <c r="S21" s="3">
         <v>10100</v>
       </c>
-      <c r="T21">
+      <c r="T21" s="3">
         <v>10800</v>
       </c>
-      <c r="U21">
+      <c r="U21" s="3">
         <v>10900</v>
       </c>
-      <c r="V21">
+      <c r="V21" s="3">
         <v>11900</v>
       </c>
-      <c r="W21">
+      <c r="W21" s="3">
         <v>12000</v>
       </c>
-      <c r="X21">
+      <c r="X21" s="3">
         <v>12200</v>
       </c>
-      <c r="Y21">
+      <c r="Y21" s="3">
         <v>12331</v>
       </c>
-      <c r="Z21">
+      <c r="Z21" s="3">
         <v>12700</v>
       </c>
-      <c r="AA21">
+      <c r="AA21" s="3">
         <v>13211</v>
       </c>
-      <c r="AB21">
+      <c r="AB21" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:28">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="6" t="s">
         <v>73</v>
       </c>
       <c r="E22" s="2">
         <v>603</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>1</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="3">
         <v>3</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="3">
         <v>13</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="3">
         <v>2100</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="3">
         <v>3700</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="3">
         <v>3800</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="3">
         <v>4500</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="3">
         <v>4700</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="3">
         <v>6700</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="3">
         <v>7700</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="3">
         <v>9100</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="3">
         <v>9700</v>
       </c>
-      <c r="R22">
+      <c r="R22" s="3">
         <v>10000</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="3">
         <v>10100</v>
       </c>
-      <c r="T22">
+      <c r="T22" s="3">
         <v>10800</v>
       </c>
-      <c r="U22">
+      <c r="U22" s="3">
         <v>10900</v>
       </c>
-      <c r="V22">
+      <c r="V22" s="3">
         <v>11900</v>
       </c>
-      <c r="W22">
+      <c r="W22" s="3">
         <v>12000</v>
       </c>
-      <c r="X22">
+      <c r="X22" s="3">
         <v>12100</v>
       </c>
-      <c r="Y22">
+      <c r="Y22" s="3">
         <v>12293</v>
       </c>
-      <c r="Z22">
+      <c r="Z22" s="3">
         <v>12656</v>
       </c>
-      <c r="AA22">
+      <c r="AA22" s="3">
         <v>13165</v>
       </c>
-      <c r="AB22">
+      <c r="AB22" s="3">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:28">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="6" t="s">
         <v>76</v>
       </c>
       <c r="E23" s="2">
         <v>46</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>1</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <v>11</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="3">
         <v>18</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="3">
         <v>150</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="3">
         <v>298</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="3">
         <v>302</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="3">
         <v>374</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="3">
         <v>497</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="3">
         <v>603</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="3">
         <v>698</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="3">
         <v>838</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="3">
         <v>906</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="3">
         <v>923</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="3">
         <v>951</v>
       </c>
-      <c r="T23">
+      <c r="T23" s="3">
         <v>1000</v>
       </c>
-      <c r="U23">
+      <c r="U23" s="3">
         <v>1100</v>
       </c>
-      <c r="V23">
+      <c r="V23" s="3">
         <v>1200</v>
       </c>
-      <c r="W23">
+      <c r="W23" s="3">
         <v>1200</v>
       </c>
-      <c r="X23">
+      <c r="X23" s="3">
         <v>1200</v>
       </c>
-      <c r="Y23">
+      <c r="Y23" s="3">
         <v>1196</v>
       </c>
-      <c r="Z23">
+      <c r="Z23" s="3">
         <v>1196</v>
       </c>
-      <c r="AA23">
+      <c r="AA23" s="3">
         <v>1298</v>
       </c>
-      <c r="AB23">
+      <c r="AB23" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:28">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>1</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="3">
         <v>18</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="3">
         <v>11</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="3">
         <v>6900</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="3">
         <v>7300</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="3">
         <v>7400</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="3">
         <v>7900</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="3">
         <v>8700</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="3">
         <v>10600</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="3">
         <v>11600</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="3">
         <v>12500</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="3">
         <v>13100</v>
       </c>
-      <c r="R24">
+      <c r="R24" s="3">
         <v>13300</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="3">
         <v>13600</v>
       </c>
-      <c r="T24">
+      <c r="T24" s="3">
         <v>14200</v>
       </c>
-      <c r="U24">
+      <c r="U24" s="3">
         <v>14300</v>
       </c>
-      <c r="V24">
+      <c r="V24" s="3">
         <v>15300</v>
       </c>
-      <c r="W24">
+      <c r="W24" s="3">
         <v>15300</v>
       </c>
-      <c r="X24">
+      <c r="X24" s="3">
         <v>15500</v>
       </c>
-      <c r="Y24">
+      <c r="Y24" s="3">
         <v>15684</v>
       </c>
-      <c r="Z24">
+      <c r="Z24" s="3">
         <v>16046</v>
       </c>
-      <c r="AA24">
+      <c r="AA24" s="3">
         <v>16570</v>
       </c>
-      <c r="AB24">
+      <c r="AB24" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:28">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>1</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="3">
         <v>13</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="3">
         <v>3</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="3">
         <v>6500</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="3">
         <v>7200</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="3">
         <v>7200</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="3">
         <v>7800</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="3">
         <v>8600</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="3">
         <v>10300</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="3">
         <v>11400</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="3">
         <v>12300</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="3">
         <v>13000</v>
       </c>
-      <c r="R25">
+      <c r="R25" s="3">
         <v>13100</v>
       </c>
-      <c r="S25">
+      <c r="S25" s="3">
         <v>13200</v>
       </c>
-      <c r="T25">
+      <c r="T25" s="3">
         <v>14000</v>
       </c>
-      <c r="U25">
+      <c r="U25" s="3">
         <v>14200</v>
       </c>
-      <c r="V25">
+      <c r="V25" s="3">
         <v>15100</v>
       </c>
-      <c r="W25">
+      <c r="W25" s="3">
         <v>15200</v>
       </c>
-      <c r="X25">
+      <c r="X25" s="3">
         <v>15300</v>
       </c>
-      <c r="Y25">
+      <c r="Y25" s="3">
         <v>15500</v>
       </c>
-      <c r="Z25">
+      <c r="Z25" s="3">
         <v>15902</v>
       </c>
-      <c r="AA25">
+      <c r="AA25" s="3">
         <v>16411</v>
       </c>
-      <c r="AB25">
+      <c r="AB25" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:28">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>1</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="3">
         <v>8</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="3">
         <v>49</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="3">
         <v>432</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="3">
         <v>511</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="3">
         <v>514</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="3">
         <v>573</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="3">
         <v>659</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="3">
         <v>851</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="3">
         <v>951</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="3">
         <v>1100</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="3">
         <v>1100</v>
       </c>
-      <c r="R26">
+      <c r="R26" s="3">
         <v>1100</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="3">
         <v>1200</v>
       </c>
-      <c r="T26">
+      <c r="T26" s="3">
         <v>1300</v>
       </c>
-      <c r="U26">
+      <c r="U26" s="3">
         <v>1300</v>
       </c>
-      <c r="V26">
+      <c r="V26" s="3">
         <v>1400</v>
       </c>
-      <c r="W26">
+      <c r="W26" s="3">
         <v>1400</v>
       </c>
-      <c r="X26">
+      <c r="X26" s="3">
         <v>1400</v>
       </c>
-      <c r="Y26">
+      <c r="Y26" s="3">
         <v>1411</v>
       </c>
-      <c r="Z26">
+      <c r="Z26" s="3">
         <v>1411</v>
       </c>
-      <c r="AA26">
+      <c r="AA26" s="3">
         <v>1511</v>
       </c>
-      <c r="AB26">
+      <c r="AB26" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:28">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3">
         <v>1</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="3">
         <v>71</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="3">
         <v>7</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="3">
         <v>5800</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="3">
         <v>7100</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="3">
         <v>7200</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="3">
         <v>7700</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="3">
         <v>8500</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="3">
         <v>10200</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="3">
         <v>11200</v>
       </c>
-      <c r="P27">
+      <c r="P27" s="3">
         <v>12200</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" s="3">
         <v>12900</v>
       </c>
-      <c r="R27">
+      <c r="R27" s="3">
         <v>13000</v>
       </c>
-      <c r="S27">
+      <c r="S27" s="3">
         <v>13300</v>
       </c>
-      <c r="T27">
+      <c r="T27" s="3">
         <v>13900</v>
       </c>
-      <c r="U27">
+      <c r="U27" s="3">
         <v>14100</v>
       </c>
-      <c r="V27">
+      <c r="V27" s="3">
         <v>15100</v>
       </c>
-      <c r="W27">
+      <c r="W27" s="3">
         <v>15100</v>
       </c>
-      <c r="X27">
+      <c r="X27" s="3">
         <v>15200</v>
       </c>
-      <c r="Y27">
+      <c r="Y27" s="3">
         <v>15403</v>
       </c>
-      <c r="Z27">
+      <c r="Z27" s="3">
         <v>15403</v>
       </c>
-      <c r="AA27">
+      <c r="AA27" s="3">
         <v>16310</v>
       </c>
-      <c r="AB27">
+      <c r="AB27" s="3">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:28">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="3">
         <v>1</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="3">
         <v>37</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="3">
         <v>64</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="3">
         <v>5900</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="3">
         <v>7200</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="3">
         <v>7200</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="3">
         <v>7700</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="3">
         <v>8500</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="3">
         <v>10200</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="3">
         <v>11200</v>
       </c>
-      <c r="P28">
+      <c r="P28" s="3">
         <v>12300</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="3">
         <v>12900</v>
       </c>
-      <c r="R28">
+      <c r="R28" s="3">
         <v>13000</v>
       </c>
-      <c r="S28">
+      <c r="S28" s="3">
         <v>13300</v>
       </c>
-      <c r="T28">
+      <c r="T28" s="3">
         <v>13900</v>
       </c>
-      <c r="U28">
+      <c r="U28" s="3">
         <v>14100</v>
       </c>
-      <c r="V28">
+      <c r="V28" s="3">
         <v>15000</v>
       </c>
-      <c r="W28">
+      <c r="W28" s="3">
         <v>15100</v>
       </c>
-      <c r="X28">
+      <c r="X28" s="3">
         <v>15200</v>
       </c>
-      <c r="Y28">
+      <c r="Y28" s="3">
         <v>15178</v>
       </c>
-      <c r="Z28">
+      <c r="Z28" s="3">
         <v>15736</v>
       </c>
-      <c r="AA28">
+      <c r="AA28" s="3">
         <v>16124</v>
       </c>
-      <c r="AB28">
+      <c r="AB28" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:28">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="3">
         <v>1</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="3">
         <v>23</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="3">
         <v>22</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="3">
         <v>5800</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="3">
         <v>7200</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="3">
         <v>7200</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="3">
         <v>7700</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="3">
         <v>8500</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="3">
         <v>10200</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="3">
         <v>11200</v>
       </c>
-      <c r="P29">
+      <c r="P29" s="3">
         <v>12200</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="3">
         <v>12900</v>
       </c>
-      <c r="R29">
+      <c r="R29" s="3">
         <v>13000</v>
       </c>
-      <c r="S29">
+      <c r="S29" s="3">
         <v>13300</v>
       </c>
-      <c r="T29">
+      <c r="T29" s="3">
         <v>13900</v>
       </c>
-      <c r="U29">
+      <c r="U29" s="3">
         <v>14000</v>
       </c>
-      <c r="V29">
+      <c r="V29" s="3">
         <v>15000</v>
       </c>
-      <c r="W29">
+      <c r="W29" s="3">
         <v>15100</v>
       </c>
-      <c r="X29">
+      <c r="X29" s="3">
         <v>15100</v>
       </c>
-      <c r="Y29">
+      <c r="Y29" s="3">
         <v>15247</v>
       </c>
-      <c r="Z29">
+      <c r="Z29" s="3">
         <v>15772</v>
       </c>
-      <c r="AA29">
+      <c r="AA29" s="3">
         <v>16200</v>
       </c>
-      <c r="AB29">
+      <c r="AB29" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:28">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="3">
         <v>14</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="3">
         <v>55</v>
       </c>
-      <c r="P30">
+      <c r="P30" s="3">
         <v>150</v>
       </c>
-      <c r="Q30" s="8">
+      <c r="Q30" s="3">
         <v>158</v>
       </c>
-      <c r="T30">
+      <c r="T30" s="3">
         <v>172</v>
       </c>
-      <c r="U30">
+      <c r="U30" s="3">
         <v>270</v>
       </c>
-      <c r="V30">
+      <c r="V30" s="3">
         <v>272</v>
       </c>
-      <c r="W30">
+      <c r="W30" s="3">
         <v>275</v>
       </c>
-      <c r="X30">
+      <c r="X30" s="3">
         <v>285</v>
       </c>
-      <c r="Y30">
+      <c r="Y30" s="3">
         <v>302</v>
       </c>
-      <c r="Z30">
+      <c r="Z30" s="3">
         <v>341</v>
       </c>
-      <c r="AA30">
+      <c r="AA30" s="3">
         <v>398</v>
       </c>
-      <c r="AB30">
+      <c r="AB30" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:28">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="3">
         <v>5</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="3">
         <v>12</v>
       </c>
-      <c r="P31" s="8">
+      <c r="P31" s="3">
         <v>129</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="3">
         <v>271</v>
       </c>
-      <c r="T31">
+      <c r="T31" s="3">
         <v>1300</v>
       </c>
-      <c r="U31">
+      <c r="U31" s="3">
         <v>1400</v>
       </c>
-      <c r="V31">
+      <c r="V31" s="3">
         <v>2300</v>
       </c>
-      <c r="W31">
+      <c r="W31" s="3">
         <v>2400</v>
       </c>
-      <c r="X31">
+      <c r="X31" s="3">
         <v>2500</v>
       </c>
-      <c r="Y31">
+      <c r="Y31" s="3">
         <v>2618</v>
       </c>
-      <c r="Z31">
+      <c r="Z31" s="3">
         <v>2618</v>
       </c>
-      <c r="AA31">
+      <c r="AA31" s="3">
         <v>3534</v>
       </c>
-      <c r="AB31">
+      <c r="AB31" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:28">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="3">
         <v>15</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="3">
         <v>45</v>
       </c>
-      <c r="P32" s="8">
+      <c r="P32" s="3">
         <v>91</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="3">
         <v>269</v>
       </c>
-      <c r="T32">
+      <c r="T32" s="3">
         <v>1300</v>
       </c>
-      <c r="U32">
+      <c r="U32" s="3">
         <v>1400</v>
       </c>
-      <c r="V32">
+      <c r="V32" s="3">
         <v>2300</v>
       </c>
-      <c r="W32">
+      <c r="W32" s="3">
         <v>2400</v>
       </c>
-      <c r="X32">
+      <c r="X32" s="3">
         <v>2500</v>
       </c>
-      <c r="Y32">
+      <c r="Y32" s="3">
         <v>2562</v>
       </c>
-      <c r="Z32">
+      <c r="Z32" s="3">
         <v>3007</v>
       </c>
-      <c r="AA32">
+      <c r="AA32" s="3">
         <v>3514</v>
       </c>
-      <c r="AB32">
+      <c r="AB32" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:28">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="3">
         <v>21</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="3">
         <v>1</v>
       </c>
-      <c r="P33" s="8">
+      <c r="P33" s="3">
         <v>110</v>
       </c>
-      <c r="Q33">
+      <c r="Q33" s="3">
         <v>201</v>
       </c>
-      <c r="T33">
+      <c r="T33" s="3">
         <v>1300</v>
       </c>
-      <c r="U33">
+      <c r="U33" s="3">
         <v>1400</v>
       </c>
-      <c r="V33">
+      <c r="V33" s="3">
         <v>2300</v>
       </c>
-      <c r="W33">
+      <c r="W33" s="3">
         <v>2400</v>
       </c>
-      <c r="X33">
+      <c r="X33" s="3">
         <v>2500</v>
       </c>
-      <c r="Y33">
+      <c r="Y33" s="3">
         <v>2665</v>
       </c>
-      <c r="Z33">
+      <c r="Z33" s="3">
         <v>2665</v>
       </c>
-      <c r="AA33">
+      <c r="AA33" s="3">
         <v>3504</v>
       </c>
-      <c r="AB33">
+      <c r="AB33" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:28">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="3">
         <v>1</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="3">
         <v>21</v>
       </c>
-      <c r="P34" s="8">
+      <c r="P34" s="3">
         <v>92</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="3">
         <v>265</v>
       </c>
-      <c r="T34">
+      <c r="T34" s="3">
         <v>1300</v>
       </c>
-      <c r="U34">
+      <c r="U34" s="3">
         <v>1400</v>
       </c>
-      <c r="V34">
+      <c r="V34" s="3">
         <v>2300</v>
       </c>
-      <c r="W34">
+      <c r="W34" s="3">
         <v>2400</v>
       </c>
-      <c r="X34">
+      <c r="X34" s="3">
         <v>2500</v>
       </c>
-      <c r="Y34">
+      <c r="Y34" s="3">
         <v>2585</v>
       </c>
-      <c r="Z34">
+      <c r="Z34" s="3">
         <v>2585</v>
       </c>
-      <c r="AA34">
+      <c r="AA34" s="3">
         <v>3492</v>
       </c>
-      <c r="AB34">
+      <c r="AB34" s="3">
         <v>0</v>
       </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
updated the files related to facebook groups
</commit_message>
<xml_diff>
--- a/Final report.xlsx
+++ b/Final report.xlsx
@@ -339,11 +339,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -373,38 +373,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,7 +389,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -435,7 +413,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -464,6 +442,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -480,22 +466,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -504,7 +474,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -532,13 +532,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,7 +628,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,85 +640,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,19 +658,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,13 +670,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -706,7 +700,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,32 +717,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -817,157 +791,183 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -983,16 +983,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1346,7 +1340,7 @@
   <dimension ref="A1:AB36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1354,7 +1348,7 @@
     <col min="1" max="1" width="19.1111111111111" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.1111111111111" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.4444444444444" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.1111111111111" style="2" customWidth="1"/>
+    <col min="4" max="4" width="80.6666666666667" style="2" customWidth="1"/>
     <col min="5" max="5" width="6.44444444444444" style="2" customWidth="1"/>
     <col min="6" max="6" width="2.22222222222222" style="3" customWidth="1"/>
     <col min="7" max="7" width="3.44444444444444" style="3" customWidth="1"/>
@@ -1398,61 +1392,61 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8">
+      <c r="I1" s="6">
         <v>44858</v>
       </c>
-      <c r="J1" s="8">
+      <c r="J1" s="6">
         <v>44859</v>
       </c>
-      <c r="K1" s="8">
+      <c r="K1" s="6">
         <v>44860</v>
       </c>
-      <c r="L1" s="8">
+      <c r="L1" s="6">
         <v>44861</v>
       </c>
-      <c r="M1" s="8">
+      <c r="M1" s="6">
         <v>44862</v>
       </c>
-      <c r="N1" s="8">
+      <c r="N1" s="6">
         <v>44865</v>
       </c>
-      <c r="O1" s="8">
+      <c r="O1" s="6">
         <v>44866</v>
       </c>
-      <c r="P1" s="8">
+      <c r="P1" s="6">
         <v>44867</v>
       </c>
-      <c r="Q1" s="8">
+      <c r="Q1" s="6">
         <v>44868</v>
       </c>
-      <c r="R1" s="8">
+      <c r="R1" s="6">
         <v>44869</v>
       </c>
-      <c r="S1" s="8">
+      <c r="S1" s="6">
         <v>44870</v>
       </c>
-      <c r="T1" s="8">
+      <c r="T1" s="6">
         <v>44872</v>
       </c>
-      <c r="U1" s="8">
+      <c r="U1" s="6">
         <v>44873</v>
       </c>
-      <c r="V1" s="8">
+      <c r="V1" s="6">
         <v>44874</v>
       </c>
-      <c r="W1" s="8">
+      <c r="W1" s="6">
         <v>44875</v>
       </c>
-      <c r="X1" s="8">
+      <c r="X1" s="6">
         <v>44876</v>
       </c>
-      <c r="Y1" s="8">
+      <c r="Y1" s="6">
         <v>44877</v>
       </c>
-      <c r="Z1" s="8">
+      <c r="Z1" s="6">
         <v>44879</v>
       </c>
-      <c r="AA1" s="8">
+      <c r="AA1" s="6">
         <v>44880</v>
       </c>
       <c r="AB1" s="1" t="s">
@@ -1460,16 +1454,16 @@
       </c>
     </row>
     <row r="2" spans="1:28">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="2">
@@ -1546,16 +1540,16 @@
       </c>
     </row>
     <row r="3" spans="1:28">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="2">
@@ -1632,16 +1626,16 @@
       </c>
     </row>
     <row r="4" spans="1:28">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="2">
@@ -1718,16 +1712,16 @@
       </c>
     </row>
     <row r="5" spans="1:28">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="2">
@@ -1804,16 +1798,16 @@
       </c>
     </row>
     <row r="6" spans="1:28">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="2">
@@ -1890,16 +1884,16 @@
       </c>
     </row>
     <row r="7" spans="1:28">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="2">
@@ -1976,16 +1970,16 @@
       </c>
     </row>
     <row r="8" spans="1:28">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="2">
@@ -2062,16 +2056,16 @@
       </c>
     </row>
     <row r="9" spans="1:28">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="2">
@@ -2148,16 +2142,16 @@
       </c>
     </row>
     <row r="10" spans="1:28">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E10" s="2">
@@ -2234,16 +2228,16 @@
       </c>
     </row>
     <row r="11" spans="1:28">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="2">
@@ -2320,16 +2314,16 @@
       </c>
     </row>
     <row r="12" spans="1:28">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="2">
@@ -2341,7 +2335,7 @@
       <c r="G12" s="3">
         <v>21</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="3" t="s">
         <v>43</v>
       </c>
       <c r="I12" s="3">
@@ -2406,16 +2400,16 @@
       </c>
     </row>
     <row r="13" spans="1:28">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E13" s="2">
@@ -2489,16 +2483,16 @@
       </c>
     </row>
     <row r="14" spans="1:28">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="2">
@@ -2575,16 +2569,16 @@
       </c>
     </row>
     <row r="15" spans="1:28">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>52</v>
       </c>
       <c r="E15" s="2">
@@ -2661,16 +2655,16 @@
       </c>
     </row>
     <row r="16" spans="1:28">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>55</v>
       </c>
       <c r="E16" s="2">
@@ -2747,16 +2741,16 @@
       </c>
     </row>
     <row r="17" spans="1:28">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>58</v>
       </c>
       <c r="E17" s="2">
@@ -2833,16 +2827,16 @@
       </c>
     </row>
     <row r="18" spans="1:28">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>61</v>
       </c>
       <c r="E18" s="2">
@@ -2919,16 +2913,16 @@
       </c>
     </row>
     <row r="19" spans="1:28">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>64</v>
       </c>
       <c r="E19" s="2">
@@ -3005,16 +2999,16 @@
       </c>
     </row>
     <row r="20" spans="1:28">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>67</v>
       </c>
       <c r="E20" s="2">
@@ -3091,16 +3085,16 @@
       </c>
     </row>
     <row r="21" spans="1:28">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>70</v>
       </c>
       <c r="E21" s="2">
@@ -3177,16 +3171,16 @@
       </c>
     </row>
     <row r="22" spans="1:28">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>73</v>
       </c>
       <c r="E22" s="2">
@@ -3263,16 +3257,16 @@
       </c>
     </row>
     <row r="23" spans="1:28">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>76</v>
       </c>
       <c r="E23" s="2">
@@ -3349,16 +3343,16 @@
       </c>
     </row>
     <row r="24" spans="1:28">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>79</v>
       </c>
       <c r="F24" s="3">
@@ -3432,16 +3426,16 @@
       </c>
     </row>
     <row r="25" spans="1:28">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F25" s="3">
@@ -3515,16 +3509,16 @@
       </c>
     </row>
     <row r="26" spans="1:28">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>85</v>
       </c>
       <c r="F26" s="3">
@@ -3598,16 +3592,16 @@
       </c>
     </row>
     <row r="27" spans="1:28">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>88</v>
       </c>
       <c r="F27" s="3">
@@ -3681,16 +3675,16 @@
       </c>
     </row>
     <row r="28" spans="1:28">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="3">
@@ -3764,16 +3758,16 @@
       </c>
     </row>
     <row r="29" spans="1:28">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>94</v>
       </c>
       <c r="F29" s="3">
@@ -3847,16 +3841,16 @@
       </c>
     </row>
     <row r="30" spans="1:28">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>96</v>
       </c>
       <c r="G30" s="3">
@@ -3900,16 +3894,16 @@
       </c>
     </row>
     <row r="31" spans="1:28">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>98</v>
       </c>
       <c r="G31" s="3">
@@ -3953,16 +3947,16 @@
       </c>
     </row>
     <row r="32" spans="1:28">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="5" t="s">
         <v>100</v>
       </c>
       <c r="G32" s="3">
@@ -4006,16 +4000,16 @@
       </c>
     </row>
     <row r="33" spans="1:28">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="5" t="s">
         <v>102</v>
       </c>
       <c r="G33" s="3">
@@ -4059,16 +4053,16 @@
       </c>
     </row>
     <row r="34" spans="1:28">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="5" t="s">
         <v>104</v>
       </c>
       <c r="G34" s="3">
@@ -4112,10 +4106,10 @@
       </c>
     </row>
     <row r="35" spans="4:4">
-      <c r="D35" s="6"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="4:4">
-      <c r="D36" s="6"/>
+      <c r="D36" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
updated group related files
</commit_message>
<xml_diff>
--- a/Final report.xlsx
+++ b/Final report.xlsx
@@ -339,11 +339,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -373,6 +373,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -380,9 +402,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -396,24 +425,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -432,13 +453,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -466,22 +480,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -494,9 +502,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -505,13 +512,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -526,19 +526,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,19 +556,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,7 +580,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,7 +592,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,7 +676,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -622,61 +688,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,25 +700,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,6 +717,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -792,17 +803,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -822,148 +822,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -986,7 +986,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1339,8 +1339,8 @@
   <sheetPr/>
   <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -4117,7 +4117,7 @@
     <hyperlink ref="D4" r:id="rId2" display="https://www.facebook.com/groups/5646866088722297/" tooltip="https://www.facebook.com/groups/5646866088722297/"/>
     <hyperlink ref="D5" r:id="rId3" display="https://www.facebook.com/groups/513992560177139/" tooltip="https://www.facebook.com/groups/513992560177139/"/>
     <hyperlink ref="D6" r:id="rId4" display="https://www.facebook.com/groups/478072124277063/" tooltip="https://www.facebook.com/groups/478072124277063/"/>
-    <hyperlink ref="D7" r:id="rId5" display="https://www.facebook.com/groups/416063824057495"/>
+    <hyperlink ref="D7" r:id="rId5" display="https://www.facebook.com/groups/416063824057495" tooltip="https://www.facebook.com/groups/416063824057495"/>
     <hyperlink ref="D16" r:id="rId6" display="https://www.facebook.com/groups/431887672302308"/>
     <hyperlink ref="D10" r:id="rId7" display="https://www.facebook.com/groups/534733661727844"/>
     <hyperlink ref="D12" r:id="rId8" display="https://www.facebook.com/groups/492319909620920"/>

</xml_diff>